<commit_message>
add png of graphs
</commit_message>
<xml_diff>
--- a/data/Fist_CorrMean_StD.xlsx
+++ b/data/Fist_CorrMean_StD.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
   <si>
     <t>Mean</t>
   </si>
@@ -29,13 +29,30 @@
   <si>
     <t>StD</t>
   </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Volunteer</t>
+  </si>
+  <si>
+    <t>MAX:</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -63,8 +80,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -77,6 +95,1003 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$4:$B$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>0.891700987855922</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.94053041361466305</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.90465227003557003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.88419970353880695</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.97284689546171499</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.86293600342592103</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.977646812328819</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.96708999929528205</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.925658967754595</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.92624183935419802</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.95208130122568102</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.95469038370881099</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.95078305997977097</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.96808272342795698</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.94755066032549995</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.81945419445130296</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.91485994374638802</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$4:$C$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>0.90824918892357098</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.95902342577939903</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.91842038454086095</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.892743308130999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.978653490318658</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.91185398908604398</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.98898457020876795</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.98208880096914697</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.96023107168447697</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.93768727828073895</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.93969535620301803</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.95727482008429798</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.97795698989548197</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.97874800741331902</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.97909939204767304</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.87216101117933797</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.94267911010781702</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$4:$D$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>0.92437524515090697</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.934097264510793</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.937752013075979</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.92338586780396503</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.97234358918351005</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.90381534317032397</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.98714836002597806</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.98150457127936497</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.94537383297949895</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.92590849680841603</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.91830847864676701</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.965875144639599</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.97292608544286496</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.97377147507017003</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.97817660450030597</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.81669863492580597</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.94514842605356397</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$4:$E$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>0.93967251360088699</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.95321279678138904</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.94529134017596605</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.960663429624944</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.96232182619227602</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.90785657416988896</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.98660411934097902</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.97662463502089403</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.90361788221651296</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.94190328624028297</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.91596515990149596</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.95659197228877701</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.971323350454526</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.96620700170863605</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.96475242382339599</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.86332819371788805</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.95963339724440999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$4:$F$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>0.91793249858083503</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.953736944478902</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.95200204384463505</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.92119177141305897</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.98685652742218699</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.96578759824605198</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.98119517188151495</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.98913495640663696</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.92717996580886697</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.94670352258628199</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.96162297864086499</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.95686361736195402</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.89960140378433795</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.96665700940015398</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.97029960988549602</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.94890902874648897</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.93719709912048399</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$G$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$G$4:$G$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>0.921009558207038</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.96404168019814496</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.92450585546710895</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.89350302425957395</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.97335348948064604</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.89748742983184004</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.98711587190836803</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.98681750222026099</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.88211935833496702</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.91544169560426403</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.96275711648955697</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.91960920807188895</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.96024688717764695</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.97944750414936599</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.968148391916826</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.82146063355515597</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.89370475596108201</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$H$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$H$4:$H$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>0.91512990159921503</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.96282547084386205</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.91694871299502001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.89399262413073599</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.97357590102898695</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.90094792146065905</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.98945697210098504</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.98698658181356402</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.87439719790860004</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.90872990706329604</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.95720759461985905</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.93959822103564505</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.95861717626688003</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.97579881757649101</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.977740054562518</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.82607780531737196</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.92188685613875399</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$I$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$I$4:$I$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>0.90563119058199404</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.95064428143701896</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.90875082962779796</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.91860197242740105</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.97606301003124896</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.993654657485605</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.99200624438621698</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.98375899324456595</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.87482944103155902</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.94358138560219296</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.97868575211328701</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.96046455197337199</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.98766190857667102</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.98257667514352798</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.97191481247747502</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.97409565241751805</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.98825363662624</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$J$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Average</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$J$4:$J$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>0.91546263556254615</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.95226403470552157</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.92604043122036728</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.91103521266618559</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.97450184113990346</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.91804243960954179</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.98626976527270371</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.98175075503121445</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.91167596471488466</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.93077467644245881</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.94829046723006638</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.95137098989554314</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.9598896076972725</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.97391115173620257</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.96971024369239878</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.86777314428885877</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.93792040312484237</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="87469056"/>
+        <c:axId val="87479040"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="87469056"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="87479040"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="87479040"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="87469056"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$J$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Average</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$J$4:$J$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>0.91546263556254615</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.95226403470552157</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.92604043122036728</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.91103521266618559</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.97450184113990346</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.91804243960954179</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.98626976527270371</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.98175075503121445</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.91167596471488466</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.93077467644245881</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.94829046723006638</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.95137098989554314</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.9598896076972725</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.97391115173620257</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.96971024369239878</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.86777314428885877</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.93792040312484237</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="143890304"/>
+        <c:axId val="144130048"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="143890304"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="144130048"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="144130048"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="143890304"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>114299</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>485774</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>85724</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -366,15 +1381,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S20"/>
+  <dimension ref="A1:T21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B3:I4"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -382,7 +1397,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -393,7 +1408,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
       <c r="B3">
         <v>1</v>
       </c>
@@ -418,6 +1436,9 @@
       <c r="I3">
         <v>8</v>
       </c>
+      <c r="J3" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="K3" t="s">
         <v>2</v>
       </c>
@@ -445,8 +1466,11 @@
       <c r="S3">
         <v>8</v>
       </c>
+      <c r="T3" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -474,6 +1498,10 @@
       <c r="I4">
         <v>0.90563119058199404</v>
       </c>
+      <c r="J4">
+        <f>AVERAGE(B4:I4)</f>
+        <v>0.91546263556254615</v>
+      </c>
       <c r="K4">
         <v>1</v>
       </c>
@@ -501,8 +1529,12 @@
       <c r="S4">
         <v>0.111477940120229</v>
       </c>
+      <c r="T4">
+        <f>AVERAGE(L4:S4)</f>
+        <v>6.3620578179794843E-2</v>
+      </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -530,6 +1562,10 @@
       <c r="I5">
         <v>0.95064428143701896</v>
       </c>
+      <c r="J5">
+        <f t="shared" ref="J5:J20" si="0">AVERAGE(B5:I5)</f>
+        <v>0.95226403470552157</v>
+      </c>
       <c r="K5">
         <v>2</v>
       </c>
@@ -557,8 +1593,12 @@
       <c r="S5">
         <v>2.3742220762685801E-2</v>
       </c>
+      <c r="T5">
+        <f t="shared" ref="T5:T20" si="1">AVERAGE(L5:S5)</f>
+        <v>2.5703543769444188E-2</v>
+      </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
@@ -586,6 +1626,10 @@
       <c r="I6">
         <v>0.90875082962779796</v>
       </c>
+      <c r="J6">
+        <f t="shared" si="0"/>
+        <v>0.92604043122036728</v>
+      </c>
       <c r="K6">
         <v>3</v>
       </c>
@@ -613,8 +1657,12 @@
       <c r="S6">
         <v>0.21230392137232099</v>
       </c>
+      <c r="T6">
+        <f t="shared" si="1"/>
+        <v>0.15639593931244963</v>
+      </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4</v>
       </c>
@@ -642,6 +1690,10 @@
       <c r="I7">
         <v>0.91860197242740105</v>
       </c>
+      <c r="J7">
+        <f t="shared" si="0"/>
+        <v>0.91103521266618559</v>
+      </c>
       <c r="K7">
         <v>4</v>
       </c>
@@ -669,8 +1721,12 @@
       <c r="S7">
         <v>3.6956467108215499E-2</v>
       </c>
+      <c r="T7">
+        <f t="shared" si="1"/>
+        <v>3.7524363052515435E-2</v>
+      </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>5</v>
       </c>
@@ -698,6 +1754,10 @@
       <c r="I8">
         <v>0.97606301003124896</v>
       </c>
+      <c r="J8">
+        <f t="shared" si="0"/>
+        <v>0.97450184113990346</v>
+      </c>
       <c r="K8">
         <v>5</v>
       </c>
@@ -725,8 +1785,12 @@
       <c r="S8">
         <v>8.00191337449975E-3</v>
       </c>
+      <c r="T8">
+        <f t="shared" si="1"/>
+        <v>7.8339614953977267E-3</v>
+      </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>6</v>
       </c>
@@ -754,6 +1818,10 @@
       <c r="I9">
         <v>0.993654657485605</v>
       </c>
+      <c r="J9">
+        <f t="shared" si="0"/>
+        <v>0.91804243960954179</v>
+      </c>
       <c r="K9">
         <v>6</v>
       </c>
@@ -781,8 +1849,12 @@
       <c r="S9">
         <v>3.6064197759348199E-3</v>
       </c>
+      <c r="T9">
+        <f t="shared" si="1"/>
+        <v>2.656032846225103E-2</v>
+      </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>7</v>
       </c>
@@ -810,6 +1882,10 @@
       <c r="I10">
         <v>0.99200624438621698</v>
       </c>
+      <c r="J10">
+        <f t="shared" si="0"/>
+        <v>0.98626976527270371</v>
+      </c>
       <c r="K10">
         <v>7</v>
       </c>
@@ -837,8 +1913,12 @@
       <c r="S10">
         <v>4.4375727751656902E-3</v>
       </c>
+      <c r="T10">
+        <f t="shared" si="1"/>
+        <v>7.3609216654685217E-3</v>
+      </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>8</v>
       </c>
@@ -866,6 +1946,10 @@
       <c r="I11">
         <v>0.98375899324456595</v>
       </c>
+      <c r="J11">
+        <f t="shared" si="0"/>
+        <v>0.98175075503121445</v>
+      </c>
       <c r="K11">
         <v>8</v>
       </c>
@@ -893,8 +1977,12 @@
       <c r="S11">
         <v>8.8602575495832694E-3</v>
       </c>
+      <c r="T11">
+        <f t="shared" si="1"/>
+        <v>8.0682565318840604E-3</v>
+      </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>9</v>
       </c>
@@ -922,6 +2010,10 @@
       <c r="I12">
         <v>0.87482944103155902</v>
       </c>
+      <c r="J12">
+        <f t="shared" si="0"/>
+        <v>0.91167596471488466</v>
+      </c>
       <c r="K12">
         <v>9</v>
       </c>
@@ -949,8 +2041,12 @@
       <c r="S12">
         <v>0.23690669473041101</v>
       </c>
+      <c r="T12">
+        <f t="shared" si="1"/>
+        <v>0.14125587691836916</v>
+      </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>10</v>
       </c>
@@ -978,6 +2074,10 @@
       <c r="I13">
         <v>0.94358138560219296</v>
       </c>
+      <c r="J13">
+        <f t="shared" si="0"/>
+        <v>0.93077467644245881</v>
+      </c>
       <c r="K13">
         <v>10</v>
       </c>
@@ -1005,8 +2105,12 @@
       <c r="S13">
         <v>0.10540118727302</v>
       </c>
+      <c r="T13">
+        <f t="shared" si="1"/>
+        <v>5.0310537643000877E-2</v>
+      </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>11</v>
       </c>
@@ -1034,6 +2138,10 @@
       <c r="I14">
         <v>0.97868575211328701</v>
       </c>
+      <c r="J14">
+        <f t="shared" si="0"/>
+        <v>0.94829046723006638</v>
+      </c>
       <c r="K14">
         <v>11</v>
       </c>
@@ -1061,8 +2169,12 @@
       <c r="S14">
         <v>8.0858153189435501E-3</v>
       </c>
+      <c r="T14">
+        <f t="shared" si="1"/>
+        <v>1.4724409601767813E-2</v>
+      </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>12</v>
       </c>
@@ -1090,6 +2202,10 @@
       <c r="I15">
         <v>0.96046455197337199</v>
       </c>
+      <c r="J15">
+        <f t="shared" si="0"/>
+        <v>0.95137098989554314</v>
+      </c>
       <c r="K15">
         <v>12</v>
       </c>
@@ -1117,8 +2233,12 @@
       <c r="S15">
         <v>9.8114125069244506E-3</v>
       </c>
+      <c r="T15">
+        <f t="shared" si="1"/>
+        <v>2.508920082286133E-2</v>
+      </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>13</v>
       </c>
@@ -1146,6 +2266,10 @@
       <c r="I16">
         <v>0.98766190857667102</v>
       </c>
+      <c r="J16">
+        <f t="shared" si="0"/>
+        <v>0.9598896076972725</v>
+      </c>
       <c r="K16">
         <v>13</v>
       </c>
@@ -1173,8 +2297,12 @@
       <c r="S16">
         <v>4.6420223892288401E-3</v>
       </c>
+      <c r="T16">
+        <f t="shared" si="1"/>
+        <v>1.038947150007353E-2</v>
+      </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>14</v>
       </c>
@@ -1202,6 +2330,10 @@
       <c r="I17">
         <v>0.98257667514352798</v>
       </c>
+      <c r="J17">
+        <f t="shared" si="0"/>
+        <v>0.97391115173620257</v>
+      </c>
       <c r="K17">
         <v>14</v>
       </c>
@@ -1229,8 +2361,12 @@
       <c r="S17">
         <v>2.1002472579193299E-2</v>
       </c>
+      <c r="T17">
+        <f t="shared" si="1"/>
+        <v>1.6812976513510453E-2</v>
+      </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>15</v>
       </c>
@@ -1258,6 +2394,10 @@
       <c r="I18">
         <v>0.97191481247747502</v>
       </c>
+      <c r="J18">
+        <f t="shared" si="0"/>
+        <v>0.96971024369239878</v>
+      </c>
       <c r="K18">
         <v>15</v>
       </c>
@@ -1285,8 +2425,12 @@
       <c r="S18">
         <v>7.6598440269124704E-3</v>
       </c>
+      <c r="T18">
+        <f t="shared" si="1"/>
+        <v>1.6290893961668069E-2</v>
+      </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>16</v>
       </c>
@@ -1314,6 +2458,10 @@
       <c r="I19">
         <v>0.97409565241751805</v>
       </c>
+      <c r="J19">
+        <f t="shared" si="0"/>
+        <v>0.86777314428885877</v>
+      </c>
       <c r="K19">
         <v>16</v>
       </c>
@@ -1341,8 +2489,12 @@
       <c r="S19">
         <v>1.67593169455247E-2</v>
       </c>
+      <c r="T19">
+        <f t="shared" si="1"/>
+        <v>3.4531581357798005E-2</v>
+      </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>17</v>
       </c>
@@ -1370,6 +2522,10 @@
       <c r="I20">
         <v>0.98825363662624</v>
       </c>
+      <c r="J20">
+        <f t="shared" si="0"/>
+        <v>0.93792040312484237</v>
+      </c>
       <c r="K20">
         <v>17</v>
       </c>
@@ -1396,10 +2552,57 @@
       </c>
       <c r="S20">
         <v>5.5946182436408002E-3</v>
+      </c>
+      <c r="T20">
+        <f t="shared" si="1"/>
+        <v>1.6148720378254645E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21">
+        <f>MAX(B4:B20)</f>
+        <v>0.977646812328819</v>
+      </c>
+      <c r="C21">
+        <f t="shared" ref="C21:J21" si="2">MAX(C4:C20)</f>
+        <v>0.98898457020876795</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="2"/>
+        <v>0.98714836002597806</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="2"/>
+        <v>0.98660411934097902</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="2"/>
+        <v>0.98913495640663696</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="2"/>
+        <v>0.98711587190836803</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="2"/>
+        <v>0.98945697210098504</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="2"/>
+        <v>0.993654657485605</v>
+      </c>
+      <c r="J21">
+        <f>MAX(J4:J20)</f>
+        <v>0.98626976527270371</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>